<commit_message>
Refactors 'Line' so that it uses the new 'Cell'. Removes all old 'Cell' logic from 'Line'. Adds a couple new tests to 'LineTest'. Fixes a couple broken tests in 'WorksheetTest' resulting from the changes above.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Line.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Line.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\excel\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7435C99-077E-4F13-ABCF-A8CE157D6166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2950B7C-D051-4702-A05B-059577454B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11145" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
+    <workbookView xWindow="28800" yWindow="6180" windowWidth="15660" windowHeight="11145" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidTinyWorkSheet" sheetId="26" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>Andrei Diego Cardoso</author>
   </authors>
   <commentList>
-    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{3B19CB41-F893-40C4-AB08-BAD30A17BF12}">
+    <comment ref="A15" authorId="0" shapeId="0" xr:uid="{3B19CB41-F893-40C4-AB08-BAD30A17BF12}">
       <text>
         <r>
           <rPr>
@@ -57,12 +57,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>String</t>
   </si>
   <si>
     <t>Note</t>
+  </si>
+  <si>
+    <t>Line with null cell</t>
+  </si>
+  <si>
+    <t>Line with blank after last non-empty</t>
   </si>
 </sst>
 </file>
@@ -448,15 +454,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5063D8FC-DCB3-4DB7-AC24-E3093A8B7A70}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -511,34 +518,45 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>1</v>
+      <c r="B11" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>78174</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B14" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6">
         <f>A2+A2</f>
         <v>156348</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adds a limit to the cells a 'Line' will read from the underlying 'XSSFRow'. As a consequence of that, validation in 'Worksheet' that prevented one from being created if any line in the underlying 'XSSFSheet' had non-empty cells beyond the limit imposed by the 'Worksheet's'Header' cannot exist in the 'Worksheet' anymore. Still, simply ignoring a non-empty cell when ingesting a 'XSSFSheet' does not sound appropriate. The user has to be notified somehow. Therefore, that validation will be moved down to the 'Line' while, at the same time, being relaxed a bit: instead of preventing a 'Line' and, consequently, the whole 'Worksheet' from being created, a warning will be logged and made available to the user in the future.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Line.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Line.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\excel\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2950B7C-D051-4702-A05B-059577454B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B4A26A7-88EF-4CF1-AA1E-C1824105150F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="6180" windowWidth="15660" windowHeight="11145" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
+    <workbookView xWindow="28770" yWindow="6285" windowWidth="15750" windowHeight="12600" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidTinyWorkSheet" sheetId="26" r:id="rId1"/>

</xml_diff>